<commit_message>
(minor) update export_liste_des_departs.xls (delete some bad rows)
</commit_message>
<xml_diff>
--- a/src/docs/asciidoc/export_liste_des_departs.xlsx
+++ b/src/docs/asciidoc/export_liste_des_departs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="262">
   <si>
     <t xml:space="preserve">mardi 6 août 2019</t>
   </si>
@@ -608,9 +608,6 @@
   </si>
   <si>
     <t xml:space="preserve">11,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAZURE Marc</t>
   </si>
   <si>
     <t xml:space="preserve">Page 2 / 3</t>
@@ -1145,15 +1142,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
+      <xdr:colOff>19800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>33120</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1166,8 +1163,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6753960" y="315720"/>
-          <a:ext cx="1143360" cy="565920"/>
+          <a:off x="6756840" y="316080"/>
+          <a:ext cx="1143720" cy="565200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1184,13 +1181,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>19080</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28080</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1203,8 +1200,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="281160" y="199440"/>
-          <a:ext cx="1252440" cy="870120"/>
+          <a:off x="281160" y="199800"/>
+          <a:ext cx="1252800" cy="869400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1219,14 +1216,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:colOff>19800</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>33120</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1240,8 +1237,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6753960" y="13091760"/>
-          <a:ext cx="1143360" cy="566280"/>
+          <a:off x="6756840" y="13070160"/>
+          <a:ext cx="1143720" cy="566280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1257,13 +1254,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19080</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28080</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1277,8 +1274,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="281160" y="12975480"/>
-          <a:ext cx="1252440" cy="870480"/>
+          <a:off x="281160" y="12953880"/>
+          <a:ext cx="1252800" cy="870480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1293,15 +1290,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:colOff>19800</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>33120</xdr:colOff>
-      <xdr:row>123</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1314,8 +1311,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6753960" y="25868160"/>
-          <a:ext cx="1143360" cy="565920"/>
+          <a:off x="6756840" y="25825320"/>
+          <a:ext cx="1143720" cy="565560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1331,14 +1328,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19080</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28080</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1351,8 +1348,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="281160" y="25751880"/>
-          <a:ext cx="1252440" cy="870120"/>
+          <a:off x="281160" y="25709040"/>
+          <a:ext cx="1252800" cy="869400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1372,10 +1369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:Q169"/>
+  <dimension ref="B1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A140" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S162" activeCellId="0" sqref="S162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1386,13 +1383,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="0.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="2.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="2.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="2.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="0.43"/>
@@ -3039,64 +3036,57 @@
       <c r="O55" s="14"/>
       <c r="P55" s="14"/>
     </row>
-    <row r="56" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-    </row>
-    <row r="57" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="10.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="15" t="s">
+    <row r="56" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="10.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="L58" s="16" t="s">
+      <c r="C57" s="15"/>
+      <c r="L57" s="16" t="s">
         <v>115</v>
       </c>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+    </row>
+    <row r="58" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L58" s="16"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
       <c r="O58" s="16"/>
       <c r="P58" s="16"/>
     </row>
-    <row r="59" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="L59" s="16"/>
-      <c r="M59" s="16"/>
-      <c r="N59" s="16"/>
-      <c r="O59" s="16"/>
-      <c r="P59" s="16"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="9.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="7.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E63" s="1" t="s">
+    <row r="59" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="9.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="7.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E62" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E65" s="2" t="s">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E64" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3105,1551 +3095,1582 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-    </row>
-    <row r="67" customFormat="false" ht="18.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="6.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="26.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="3" t="s">
+    <row r="66" customFormat="false" ht="18.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="6.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="26.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B68" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
-      <c r="O69" s="3"/>
-      <c r="P69" s="3"/>
-    </row>
-    <row r="70" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="1" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+    </row>
+    <row r="69" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-    </row>
-    <row r="71" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="4" t="s">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B70" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="5" t="s">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G70" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H70" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I70" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J71" s="5" t="s">
+      <c r="J70" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K71" s="6" t="s">
+      <c r="K70" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="4" t="s">
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P71" s="4"/>
-    </row>
-    <row r="72" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="7"/>
-    </row>
-    <row r="73" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="8" t="s">
+      <c r="P70" s="4"/>
+    </row>
+    <row r="71" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B72" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="9" t="n">
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="9" t="n">
         <v>23603764</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G72" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="H73" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I73" s="9" t="s">
+      <c r="H72" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I72" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="J73" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K73" s="10" t="s">
+      <c r="J72" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L73" s="10"/>
-      <c r="M73" s="10"/>
-      <c r="N73" s="10"/>
-      <c r="Q73" s="17" t="str">
-        <f aca="false">A73 &amp; CHAR(10) &amp; A74 &amp; CHAR(10) &amp; A75</f>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+      <c r="Q72" s="17" t="str">
+        <f aca="false">A72 &amp; CHAR(10) &amp; A73 &amp; CHAR(10) &amp; A74</f>
         <v>
 </v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B73" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="12" t="n">
+        <v>465773058</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J73" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+    </row>
     <row r="74" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="12" t="n">
-        <v>465773058</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H74" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I74" s="12" t="s">
+      <c r="B74" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="9" t="n">
+        <v>327762257</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="J74" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="13" t="s">
+      <c r="J74" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+    </row>
+    <row r="75" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B75" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="12" t="n">
+        <v>270298501</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J75" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K75" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+    </row>
+    <row r="76" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B76" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="9" t="n">
+        <v>35056541</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="J76" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+      <c r="N76" s="10"/>
+    </row>
+    <row r="77" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B77" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="12" t="n">
+        <v>385268295</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J77" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+    </row>
+    <row r="78" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B78" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="9" t="n">
+        <v>409477900</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="J78" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K78" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+    </row>
+    <row r="79" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B79" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="12" t="n">
+        <v>337648605</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I79" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J79" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K79" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+      <c r="N79" s="13"/>
+      <c r="O79" s="14"/>
+      <c r="P79" s="14"/>
+    </row>
+    <row r="80" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B80" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="9" t="n">
+        <v>336526586</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H80" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J80" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K80" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L80" s="10"/>
+      <c r="M80" s="10"/>
+      <c r="N80" s="10"/>
+    </row>
+    <row r="81" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B81" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="12" t="n">
+        <v>327671687</v>
+      </c>
+      <c r="G81" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J81" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K81" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="14"/>
+    </row>
+    <row r="82" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B82" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="9" t="n">
+        <v>435205645</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H82" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J82" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K82" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
+      <c r="N82" s="10"/>
+    </row>
+    <row r="83" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B83" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="12" t="n">
+        <v>304815304</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J83" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K83" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="14"/>
-      <c r="P74" s="14"/>
-    </row>
-    <row r="75" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="9" t="n">
-        <v>327762257</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="H75" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I75" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="10" t="s">
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
+      <c r="O83" s="14"/>
+      <c r="P83" s="14"/>
+    </row>
+    <row r="84" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B84" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="9" t="n">
+        <v>472723188</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H84" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J84" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+    </row>
+    <row r="85" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B85" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="12" t="n">
+        <v>402711429</v>
+      </c>
+      <c r="G85" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J85" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K85" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="14"/>
+      <c r="P85" s="14"/>
+    </row>
+    <row r="86" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B86" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="9" t="n">
+        <v>374336981</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J86" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K86" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L86" s="10"/>
+      <c r="M86" s="10"/>
+      <c r="N86" s="10"/>
+    </row>
+    <row r="87" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B87" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="12" t="n">
+        <v>350819677</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J87" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K87" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="L87" s="13"/>
+      <c r="M87" s="13"/>
+      <c r="N87" s="13"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="14"/>
+    </row>
+    <row r="88" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B88" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="9" t="n">
+        <v>264981500</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H88" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J88" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K88" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+    </row>
+    <row r="89" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="12" t="n">
+        <v>464397648</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J89" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K89" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="L89" s="13"/>
+      <c r="M89" s="13"/>
+      <c r="N89" s="13"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="14"/>
+    </row>
+    <row r="90" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B90" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="9" t="n">
+        <v>409586883</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J90" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+    </row>
+    <row r="91" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B91" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="12" t="n">
+        <v>287485868</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J91" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K91" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="L75" s="10"/>
-      <c r="M75" s="10"/>
-      <c r="N75" s="10"/>
-    </row>
-    <row r="76" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="12" t="n">
-        <v>270298501</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="H76" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I76" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J76" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="14"/>
-      <c r="P76" s="14"/>
-    </row>
-    <row r="77" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="9" t="n">
-        <v>35056541</v>
-      </c>
-      <c r="G77" s="9" t="s">
+      <c r="L91" s="13"/>
+      <c r="M91" s="13"/>
+      <c r="N91" s="13"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="14"/>
+    </row>
+    <row r="92" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B92" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="9" t="n">
+        <v>307650488</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J92" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K92" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="L92" s="10"/>
+      <c r="M92" s="10"/>
+      <c r="N92" s="10"/>
+    </row>
+    <row r="93" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B93" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="12" t="n">
+        <v>37603647</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J93" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K93" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="L93" s="13"/>
+      <c r="M93" s="13"/>
+      <c r="N93" s="13"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="14"/>
+    </row>
+    <row r="94" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B94" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="9" t="n">
+        <v>344885193</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J94" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K94" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+    </row>
+    <row r="95" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B95" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="12" t="n">
+        <v>504440679</v>
+      </c>
+      <c r="G95" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J95" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K95" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="L95" s="13"/>
+      <c r="M95" s="13"/>
+      <c r="N95" s="13"/>
+      <c r="O95" s="14"/>
+      <c r="P95" s="14"/>
+    </row>
+    <row r="96" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B96" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="9" t="n">
+        <v>428789221</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J96" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K96" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L96" s="10"/>
+      <c r="M96" s="10"/>
+      <c r="N96" s="10"/>
+    </row>
+    <row r="97" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B97" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="12" t="n">
+        <v>384750050</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J97" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K97" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L97" s="13"/>
+      <c r="M97" s="13"/>
+      <c r="N97" s="13"/>
+      <c r="O97" s="14"/>
+      <c r="P97" s="14"/>
+    </row>
+    <row r="98" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B98" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="9" t="n">
+        <v>382382992</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J98" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K98" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+    </row>
+    <row r="99" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B99" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="12" t="n">
+        <v>372479473</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J99" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K99" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="L99" s="13"/>
+      <c r="M99" s="13"/>
+      <c r="N99" s="13"/>
+      <c r="O99" s="14"/>
+      <c r="P99" s="14"/>
+    </row>
+    <row r="100" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B100" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="9" t="n">
+        <v>475606995</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J100" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K100" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="L100" s="10"/>
+      <c r="M100" s="10"/>
+      <c r="N100" s="10"/>
+    </row>
+    <row r="101" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B101" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="12" t="n">
+        <v>305086708</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J101" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K101" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="L101" s="13"/>
+      <c r="M101" s="13"/>
+      <c r="N101" s="13"/>
+      <c r="O101" s="14"/>
+      <c r="P101" s="14"/>
+    </row>
+    <row r="102" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B102" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="9" t="n">
+        <v>2800201</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H102" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J102" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K102" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L102" s="10"/>
+      <c r="M102" s="10"/>
+      <c r="N102" s="10"/>
+    </row>
+    <row r="103" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B103" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="12" t="n">
+        <v>362948648</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J103" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K103" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L103" s="13"/>
+      <c r="M103" s="13"/>
+      <c r="N103" s="13"/>
+      <c r="O103" s="14"/>
+      <c r="P103" s="14"/>
+    </row>
+    <row r="104" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B104" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="9" t="n">
+        <v>475564115</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H104" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J104" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K104" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L104" s="10"/>
+      <c r="M104" s="10"/>
+      <c r="N104" s="10"/>
+    </row>
+    <row r="105" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B105" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="12" t="n">
+        <v>335697634</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="H105" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J105" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K105" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L105" s="13"/>
+      <c r="M105" s="13"/>
+      <c r="N105" s="13"/>
+      <c r="O105" s="14"/>
+      <c r="P105" s="14"/>
+    </row>
+    <row r="106" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B106" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="9" t="n">
+        <v>457599934</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H106" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J106" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K106" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L106" s="10"/>
+      <c r="M106" s="10"/>
+      <c r="N106" s="10"/>
+    </row>
+    <row r="107" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B107" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="12" t="n">
+        <v>445726459</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J107" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K107" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L107" s="13"/>
+      <c r="M107" s="13"/>
+      <c r="N107" s="13"/>
+      <c r="O107" s="14"/>
+      <c r="P107" s="14"/>
+    </row>
+    <row r="108" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B108" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="9" t="n">
+        <v>389713917</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H108" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J108" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K108" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="L108" s="10"/>
+      <c r="M108" s="10"/>
+      <c r="N108" s="10"/>
+    </row>
+    <row r="109" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B109" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="12" t="n">
+        <v>361918450</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="H109" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J109" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K109" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L109" s="13"/>
+      <c r="M109" s="13"/>
+      <c r="N109" s="13"/>
+      <c r="O109" s="14"/>
+      <c r="P109" s="14"/>
+    </row>
+    <row r="110" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B110" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="9" t="n">
+        <v>344873411</v>
+      </c>
+      <c r="G110" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="H77" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="J77" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K77" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L77" s="10"/>
-      <c r="M77" s="10"/>
-      <c r="N77" s="10"/>
-    </row>
-    <row r="78" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="12" t="n">
-        <v>385268295</v>
-      </c>
-      <c r="G78" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I78" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J78" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K78" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="14"/>
-      <c r="P78" s="14"/>
-    </row>
-    <row r="79" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="9" t="n">
-        <v>409477900</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H79" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I79" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="J79" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K79" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="L79" s="10"/>
-      <c r="M79" s="10"/>
-      <c r="N79" s="10"/>
-    </row>
-    <row r="80" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="12" t="n">
-        <v>337648605</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H80" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="I80" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J80" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K80" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="14"/>
-      <c r="P80" s="14"/>
-    </row>
-    <row r="81" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="9" t="n">
-        <v>336526586</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="H81" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I81" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J81" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K81" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L81" s="10"/>
-      <c r="M81" s="10"/>
-      <c r="N81" s="10"/>
-    </row>
-    <row r="82" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="12" t="n">
-        <v>327671687</v>
-      </c>
-      <c r="G82" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="H82" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I82" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J82" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K82" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="L82" s="13"/>
-      <c r="M82" s="13"/>
-      <c r="N82" s="13"/>
-      <c r="O82" s="14"/>
-      <c r="P82" s="14"/>
-    </row>
-    <row r="83" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="9" t="n">
-        <v>435205645</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H83" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I83" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J83" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K83" s="10" t="s">
+      <c r="H110" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J110" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K110" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="L110" s="10"/>
+      <c r="M110" s="10"/>
+      <c r="N110" s="10"/>
+    </row>
+    <row r="111" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B111" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="12" t="n">
+        <v>438307021</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J111" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K111" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10"/>
-    </row>
-    <row r="84" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="12" t="n">
-        <v>304815304</v>
-      </c>
-      <c r="G84" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="H84" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J84" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="14"/>
-      <c r="P84" s="14"/>
-    </row>
-    <row r="85" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="9" t="n">
-        <v>472723188</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="H85" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J85" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K85" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="L85" s="10"/>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10"/>
-    </row>
-    <row r="86" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="12" t="n">
-        <v>402711429</v>
-      </c>
-      <c r="G86" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="H86" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I86" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J86" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K86" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-      <c r="N86" s="13"/>
-      <c r="O86" s="14"/>
-      <c r="P86" s="14"/>
-    </row>
-    <row r="87" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="9" t="n">
-        <v>374336981</v>
-      </c>
-      <c r="G87" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H87" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I87" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J87" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K87" s="10" t="s">
+      <c r="L111" s="13"/>
+      <c r="M111" s="13"/>
+      <c r="N111" s="13"/>
+      <c r="O111" s="14"/>
+      <c r="P111" s="14"/>
+    </row>
+    <row r="112" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B112" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="9" t="n">
+        <v>36511688</v>
+      </c>
+      <c r="G112" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J112" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K112" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="L112" s="10"/>
+      <c r="M112" s="10"/>
+      <c r="N112" s="10"/>
+    </row>
+    <row r="113" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B113" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="12" t="n">
+        <v>469263901</v>
+      </c>
+      <c r="G113" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I113" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J113" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K113" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="L113" s="13"/>
+      <c r="M113" s="13"/>
+      <c r="N113" s="13"/>
+      <c r="O113" s="14"/>
+      <c r="P113" s="14"/>
+    </row>
+    <row r="114" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="10.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B115" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C115" s="15"/>
+      <c r="L115" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="M115" s="16"/>
+      <c r="N115" s="16"/>
+      <c r="O115" s="16"/>
+      <c r="P115" s="16"/>
+    </row>
+    <row r="116" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L116" s="16"/>
+      <c r="M116" s="16"/>
+      <c r="N116" s="16"/>
+      <c r="O116" s="16"/>
+      <c r="P116" s="16"/>
+    </row>
+    <row r="117" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="9.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="7.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E122" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+    </row>
+    <row r="123" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+    </row>
+    <row r="124" customFormat="false" ht="18.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="6.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="26.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B126" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="3"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+      <c r="P126" s="3"/>
+    </row>
+    <row r="127" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+      <c r="N127" s="1"/>
+      <c r="O127" s="1"/>
+      <c r="P127" s="1"/>
+    </row>
+    <row r="128" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B128" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H128" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K128" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L128" s="6"/>
+      <c r="M128" s="6"/>
+      <c r="N128" s="6"/>
+      <c r="O128" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P128" s="4"/>
+    </row>
+    <row r="129" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7"/>
+      <c r="G129" s="7"/>
+      <c r="H129" s="7"/>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="M129" s="7"/>
+      <c r="N129" s="7"/>
+      <c r="O129" s="7"/>
+      <c r="P129" s="7"/>
+    </row>
+    <row r="130" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B130" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="9" t="n">
+        <v>372748977</v>
+      </c>
+      <c r="G130" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H130" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I130" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J130" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K130" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L87" s="10"/>
-      <c r="M87" s="10"/>
-      <c r="N87" s="10"/>
-    </row>
-    <row r="88" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="12" t="n">
-        <v>350819677</v>
-      </c>
-      <c r="G88" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="H88" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I88" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J88" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K88" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="L88" s="13"/>
-      <c r="M88" s="13"/>
-      <c r="N88" s="13"/>
-      <c r="O88" s="14"/>
-      <c r="P88" s="14"/>
-    </row>
-    <row r="89" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="9" t="n">
-        <v>264981500</v>
-      </c>
-      <c r="G89" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H89" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J89" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K89" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="L89" s="10"/>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10"/>
-    </row>
-    <row r="90" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="12" t="n">
-        <v>464397648</v>
-      </c>
-      <c r="G90" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="H90" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I90" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J90" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K90" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13"/>
-      <c r="N90" s="13"/>
-      <c r="O90" s="14"/>
-      <c r="P90" s="14"/>
-    </row>
-    <row r="91" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="9" t="n">
-        <v>409586883</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I91" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J91" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L91" s="10"/>
-      <c r="M91" s="10"/>
-      <c r="N91" s="10"/>
-    </row>
-    <row r="92" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="12" t="n">
-        <v>287485868</v>
-      </c>
-      <c r="G92" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="H92" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I92" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J92" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
-      <c r="N92" s="13"/>
-      <c r="O92" s="14"/>
-      <c r="P92" s="14"/>
-    </row>
-    <row r="93" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="9" t="n">
-        <v>307650488</v>
-      </c>
-      <c r="G93" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="H93" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I93" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J93" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K93" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="L93" s="10"/>
-      <c r="M93" s="10"/>
-      <c r="N93" s="10"/>
-    </row>
-    <row r="94" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="12" t="n">
-        <v>37603647</v>
-      </c>
-      <c r="G94" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="H94" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I94" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J94" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K94" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13"/>
-      <c r="N94" s="13"/>
-      <c r="O94" s="14"/>
-      <c r="P94" s="14"/>
-    </row>
-    <row r="95" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="9" t="n">
-        <v>344885193</v>
-      </c>
-      <c r="G95" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="H95" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J95" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K95" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="L95" s="10"/>
-      <c r="M95" s="10"/>
-      <c r="N95" s="10"/>
-    </row>
-    <row r="96" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="12" t="n">
-        <v>504440679</v>
-      </c>
-      <c r="G96" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I96" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J96" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K96" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="L96" s="13"/>
-      <c r="M96" s="13"/>
-      <c r="N96" s="13"/>
-      <c r="O96" s="14"/>
-      <c r="P96" s="14"/>
-    </row>
-    <row r="97" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="9" t="n">
-        <v>428789221</v>
-      </c>
-      <c r="G97" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H97" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I97" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J97" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K97" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L97" s="10"/>
-      <c r="M97" s="10"/>
-      <c r="N97" s="10"/>
-    </row>
-    <row r="98" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="12" t="n">
-        <v>384750050</v>
-      </c>
-      <c r="G98" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J98" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K98" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
-      <c r="N98" s="13"/>
-      <c r="O98" s="14"/>
-      <c r="P98" s="14"/>
-    </row>
-    <row r="99" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="9" t="n">
-        <v>382382992</v>
-      </c>
-      <c r="G99" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H99" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I99" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J99" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K99" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L99" s="10"/>
-      <c r="M99" s="10"/>
-      <c r="N99" s="10"/>
-    </row>
-    <row r="100" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="12" t="n">
-        <v>372479473</v>
-      </c>
-      <c r="G100" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H100" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I100" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J100" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K100" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="L100" s="13"/>
-      <c r="M100" s="13"/>
-      <c r="N100" s="13"/>
-      <c r="O100" s="14"/>
-      <c r="P100" s="14"/>
-    </row>
-    <row r="101" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="9" t="n">
-        <v>475606995</v>
-      </c>
-      <c r="G101" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H101" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I101" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J101" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K101" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="L101" s="10"/>
-      <c r="M101" s="10"/>
-      <c r="N101" s="10"/>
-    </row>
-    <row r="102" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="12" t="n">
-        <v>305086708</v>
-      </c>
-      <c r="G102" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H102" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I102" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J102" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K102" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="L102" s="13"/>
-      <c r="M102" s="13"/>
-      <c r="N102" s="13"/>
-      <c r="O102" s="14"/>
-      <c r="P102" s="14"/>
-    </row>
-    <row r="103" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="9" t="n">
-        <v>2800201</v>
-      </c>
-      <c r="G103" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H103" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I103" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J103" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K103" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L103" s="10"/>
-      <c r="M103" s="10"/>
-      <c r="N103" s="10"/>
-    </row>
-    <row r="104" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="12" t="n">
-        <v>362948648</v>
-      </c>
-      <c r="G104" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I104" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J104" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K104" s="13" t="s">
+      <c r="L130" s="10"/>
+      <c r="M130" s="10"/>
+      <c r="N130" s="10"/>
+    </row>
+    <row r="131" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B131" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="11"/>
+      <c r="F131" s="12" t="n">
+        <v>362397202</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="H131" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I131" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J131" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K131" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="L104" s="13"/>
-      <c r="M104" s="13"/>
-      <c r="N104" s="13"/>
-      <c r="O104" s="14"/>
-      <c r="P104" s="14"/>
-    </row>
-    <row r="105" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="9" t="n">
-        <v>475564115</v>
-      </c>
-      <c r="G105" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H105" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J105" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K105" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L105" s="10"/>
-      <c r="M105" s="10"/>
-      <c r="N105" s="10"/>
-    </row>
-    <row r="106" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="12" t="n">
-        <v>335697634</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="H106" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I106" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J106" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K106" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="L106" s="13"/>
-      <c r="M106" s="13"/>
-      <c r="N106" s="13"/>
-      <c r="O106" s="14"/>
-      <c r="P106" s="14"/>
-    </row>
-    <row r="107" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="9" t="n">
-        <v>457599934</v>
-      </c>
-      <c r="G107" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="H107" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I107" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J107" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K107" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="L107" s="10"/>
-      <c r="M107" s="10"/>
-      <c r="N107" s="10"/>
-    </row>
-    <row r="108" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="12" t="n">
-        <v>445726459</v>
-      </c>
-      <c r="G108" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="H108" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I108" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J108" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K108" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L108" s="13"/>
-      <c r="M108" s="13"/>
-      <c r="N108" s="13"/>
-      <c r="O108" s="14"/>
-      <c r="P108" s="14"/>
-    </row>
-    <row r="109" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="9" t="n">
-        <v>389713917</v>
-      </c>
-      <c r="G109" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H109" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I109" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J109" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K109" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="L109" s="10"/>
-      <c r="M109" s="10"/>
-      <c r="N109" s="10"/>
-    </row>
-    <row r="110" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="12" t="n">
-        <v>361918450</v>
-      </c>
-      <c r="G110" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="H110" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I110" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J110" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K110" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="L110" s="13"/>
-      <c r="M110" s="13"/>
-      <c r="N110" s="13"/>
-      <c r="O110" s="14"/>
-      <c r="P110" s="14"/>
-    </row>
-    <row r="111" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="9" t="n">
-        <v>344873411</v>
-      </c>
-      <c r="G111" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="H111" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I111" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J111" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K111" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="L111" s="10"/>
-      <c r="M111" s="10"/>
-      <c r="N111" s="10"/>
-    </row>
-    <row r="112" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="12" t="n">
-        <v>438307021</v>
-      </c>
-      <c r="G112" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="H112" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I112" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J112" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K112" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L112" s="13"/>
-      <c r="M112" s="13"/>
-      <c r="N112" s="13"/>
-      <c r="O112" s="14"/>
-      <c r="P112" s="14"/>
-    </row>
-    <row r="113" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="9" t="n">
-        <v>36511688</v>
-      </c>
-      <c r="G113" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="H113" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I113" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J113" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K113" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="L113" s="10"/>
-      <c r="M113" s="10"/>
-      <c r="N113" s="10"/>
-    </row>
-    <row r="114" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="12" t="n">
-        <v>469263901</v>
-      </c>
-      <c r="G114" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="H114" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I114" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J114" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K114" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="L114" s="13"/>
-      <c r="M114" s="13"/>
-      <c r="N114" s="13"/>
-      <c r="O114" s="14"/>
-      <c r="P114" s="14"/>
-    </row>
-    <row r="115" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="C115" s="7"/>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="7"/>
-      <c r="G115" s="7"/>
-      <c r="H115" s="7"/>
-      <c r="I115" s="7"/>
-      <c r="J115" s="7"/>
-      <c r="K115" s="7"/>
-      <c r="L115" s="7"/>
-      <c r="M115" s="7"/>
-      <c r="N115" s="7"/>
-      <c r="O115" s="7"/>
-      <c r="P115" s="7"/>
-    </row>
-    <row r="116" customFormat="false" ht="22.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="10.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C117" s="15"/>
-      <c r="L117" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="M117" s="16"/>
-      <c r="N117" s="16"/>
-      <c r="O117" s="16"/>
-      <c r="P117" s="16"/>
-    </row>
-    <row r="118" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="L118" s="16"/>
-      <c r="M118" s="16"/>
-      <c r="N118" s="16"/>
-      <c r="O118" s="16"/>
-      <c r="P118" s="16"/>
-    </row>
-    <row r="119" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="9.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="7.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E122" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1"/>
-      <c r="J122" s="1"/>
-      <c r="K122" s="1"/>
-      <c r="L122" s="1"/>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E124" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
-      <c r="L124" s="2"/>
-    </row>
-    <row r="125" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
-      <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
-      <c r="J125" s="2"/>
-      <c r="K125" s="2"/>
-      <c r="L125" s="2"/>
-    </row>
-    <row r="126" customFormat="false" ht="18.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="6.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="26.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="3"/>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="3"/>
-      <c r="K128" s="3"/>
-      <c r="L128" s="3"/>
-      <c r="M128" s="3"/>
-      <c r="N128" s="3"/>
-      <c r="O128" s="3"/>
-      <c r="P128" s="3"/>
-    </row>
-    <row r="129" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
-      <c r="G129" s="1"/>
-      <c r="H129" s="1"/>
-      <c r="I129" s="1"/>
-      <c r="J129" s="1"/>
-      <c r="K129" s="1"/>
-      <c r="L129" s="1"/>
-      <c r="M129" s="1"/>
-      <c r="N129" s="1"/>
-      <c r="O129" s="1"/>
-      <c r="P129" s="1"/>
-    </row>
-    <row r="130" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="4"/>
-      <c r="F130" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G130" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H130" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I130" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J130" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K130" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L130" s="6"/>
-      <c r="M130" s="6"/>
-      <c r="N130" s="6"/>
-      <c r="O130" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P130" s="4"/>
-    </row>
-    <row r="131" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
-      <c r="F131" s="7"/>
-      <c r="G131" s="7"/>
-      <c r="H131" s="7"/>
-      <c r="I131" s="7"/>
-      <c r="J131" s="7"/>
-      <c r="K131" s="7"/>
-      <c r="L131" s="7"/>
-      <c r="M131" s="7"/>
-      <c r="N131" s="7"/>
-      <c r="O131" s="7"/>
-      <c r="P131" s="7"/>
+      <c r="L131" s="13"/>
+      <c r="M131" s="13"/>
+      <c r="N131" s="13"/>
+      <c r="O131" s="14"/>
+      <c r="P131" s="14"/>
     </row>
     <row r="132" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="8" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
       <c r="E132" s="8"/>
       <c r="F132" s="9" t="n">
-        <v>372748977</v>
+        <v>29222195</v>
       </c>
       <c r="G132" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H132" s="10" t="s">
         <v>14</v>
@@ -4661,7 +4682,7 @@
         <v>16</v>
       </c>
       <c r="K132" s="10" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
       <c r="L132" s="10"/>
       <c r="M132" s="10"/>
@@ -4669,16 +4690,16 @@
     </row>
     <row r="133" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="11" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
       <c r="F133" s="12" t="n">
-        <v>362397202</v>
+        <v>45186958</v>
       </c>
       <c r="G133" s="12" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H133" s="13" t="s">
         <v>14</v>
@@ -4690,7 +4711,7 @@
         <v>16</v>
       </c>
       <c r="K133" s="13" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
       <c r="L133" s="13"/>
       <c r="M133" s="13"/>
@@ -4700,16 +4721,16 @@
     </row>
     <row r="134" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="8" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
       <c r="E134" s="8"/>
       <c r="F134" s="9" t="n">
-        <v>29222195</v>
+        <v>274073584</v>
       </c>
       <c r="G134" s="9" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H134" s="10" t="s">
         <v>14</v>
@@ -4718,10 +4739,10 @@
         <v>15</v>
       </c>
       <c r="J134" s="9" t="s">
-        <v>16</v>
+        <v>208</v>
       </c>
       <c r="K134" s="10" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="L134" s="10"/>
       <c r="M134" s="10"/>
@@ -4729,16 +4750,16 @@
     </row>
     <row r="135" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="11" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
       <c r="F135" s="12" t="n">
-        <v>45186958</v>
+        <v>410884496</v>
       </c>
       <c r="G135" s="12" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="H135" s="13" t="s">
         <v>14</v>
@@ -4750,7 +4771,7 @@
         <v>16</v>
       </c>
       <c r="K135" s="13" t="s">
-        <v>206</v>
+        <v>30</v>
       </c>
       <c r="L135" s="13"/>
       <c r="M135" s="13"/>
@@ -4760,16 +4781,16 @@
     </row>
     <row r="136" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="8" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
       <c r="F136" s="9" t="n">
-        <v>274073584</v>
+        <v>344363071</v>
       </c>
       <c r="G136" s="9" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="H136" s="10" t="s">
         <v>14</v>
@@ -4778,10 +4799,10 @@
         <v>15</v>
       </c>
       <c r="J136" s="9" t="s">
-        <v>209</v>
+        <v>16</v>
       </c>
       <c r="K136" s="10" t="s">
-        <v>210</v>
+        <v>69</v>
       </c>
       <c r="L136" s="10"/>
       <c r="M136" s="10"/>
@@ -4789,16 +4810,16 @@
     </row>
     <row r="137" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="11" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C137" s="11"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
       <c r="F137" s="12" t="n">
-        <v>410884496</v>
+        <v>357578438</v>
       </c>
       <c r="G137" s="12" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="H137" s="13" t="s">
         <v>14</v>
@@ -4810,7 +4831,7 @@
         <v>16</v>
       </c>
       <c r="K137" s="13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L137" s="13"/>
       <c r="M137" s="13"/>
@@ -4820,16 +4841,16 @@
     </row>
     <row r="138" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="8" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
       <c r="F138" s="9" t="n">
-        <v>344363071</v>
+        <v>398054015</v>
       </c>
       <c r="G138" s="9" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H138" s="10" t="s">
         <v>14</v>
@@ -4841,7 +4862,7 @@
         <v>16</v>
       </c>
       <c r="K138" s="10" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="L138" s="10"/>
       <c r="M138" s="10"/>
@@ -4849,16 +4870,16 @@
     </row>
     <row r="139" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="11" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="12" t="n">
-        <v>357578438</v>
+        <v>35073897</v>
       </c>
       <c r="G139" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H139" s="13" t="s">
         <v>14</v>
@@ -4880,16 +4901,16 @@
     </row>
     <row r="140" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="8" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
       <c r="E140" s="8"/>
       <c r="F140" s="9" t="n">
-        <v>398054015</v>
+        <v>362847677</v>
       </c>
       <c r="G140" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H140" s="10" t="s">
         <v>14</v>
@@ -4901,7 +4922,7 @@
         <v>16</v>
       </c>
       <c r="K140" s="10" t="s">
-        <v>53</v>
+        <v>221</v>
       </c>
       <c r="L140" s="10"/>
       <c r="M140" s="10"/>
@@ -4909,16 +4930,16 @@
     </row>
     <row r="141" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="11" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C141" s="11"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="12" t="n">
-        <v>35073897</v>
+        <v>381720414</v>
       </c>
       <c r="G141" s="12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H141" s="13" t="s">
         <v>14</v>
@@ -4930,7 +4951,7 @@
         <v>16</v>
       </c>
       <c r="K141" s="13" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="L141" s="13"/>
       <c r="M141" s="13"/>
@@ -4940,16 +4961,16 @@
     </row>
     <row r="142" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="8" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
       <c r="F142" s="9" t="n">
-        <v>362847677</v>
+        <v>452332771</v>
       </c>
       <c r="G142" s="9" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="H142" s="10" t="s">
         <v>14</v>
@@ -4961,7 +4982,7 @@
         <v>16</v>
       </c>
       <c r="K142" s="10" t="s">
-        <v>222</v>
+        <v>63</v>
       </c>
       <c r="L142" s="10"/>
       <c r="M142" s="10"/>
@@ -4969,16 +4990,16 @@
     </row>
     <row r="143" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="11" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
       <c r="F143" s="12" t="n">
-        <v>381720414</v>
+        <v>312388889</v>
       </c>
       <c r="G143" s="12" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="H143" s="13" t="s">
         <v>14</v>
@@ -4990,7 +5011,7 @@
         <v>16</v>
       </c>
       <c r="K143" s="13" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="L143" s="13"/>
       <c r="M143" s="13"/>
@@ -5000,16 +5021,16 @@
     </row>
     <row r="144" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="8" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
       <c r="E144" s="8"/>
       <c r="F144" s="9" t="n">
-        <v>452332771</v>
+        <v>444508552</v>
       </c>
       <c r="G144" s="9" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H144" s="10" t="s">
         <v>14</v>
@@ -5021,7 +5042,7 @@
         <v>16</v>
       </c>
       <c r="K144" s="10" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="L144" s="10"/>
       <c r="M144" s="10"/>
@@ -5029,16 +5050,16 @@
     </row>
     <row r="145" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="11" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C145" s="11"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
       <c r="F145" s="12" t="n">
-        <v>312388889</v>
+        <v>346986259</v>
       </c>
       <c r="G145" s="12" t="s">
-        <v>227</v>
+        <v>122</v>
       </c>
       <c r="H145" s="13" t="s">
         <v>14</v>
@@ -5050,7 +5071,7 @@
         <v>16</v>
       </c>
       <c r="K145" s="13" t="s">
-        <v>24</v>
+        <v>230</v>
       </c>
       <c r="L145" s="13"/>
       <c r="M145" s="13"/>
@@ -5060,16 +5081,16 @@
     </row>
     <row r="146" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="8" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
       <c r="E146" s="8"/>
       <c r="F146" s="9" t="n">
-        <v>444508552</v>
+        <v>273104907</v>
       </c>
       <c r="G146" s="9" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H146" s="10" t="s">
         <v>14</v>
@@ -5081,7 +5102,7 @@
         <v>16</v>
       </c>
       <c r="K146" s="10" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="L146" s="10"/>
       <c r="M146" s="10"/>
@@ -5089,16 +5110,16 @@
     </row>
     <row r="147" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="11" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C147" s="11"/>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
       <c r="F147" s="12" t="n">
-        <v>346986259</v>
+        <v>485444948</v>
       </c>
       <c r="G147" s="12" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="H147" s="13" t="s">
         <v>14</v>
@@ -5110,7 +5131,7 @@
         <v>16</v>
       </c>
       <c r="K147" s="13" t="s">
-        <v>231</v>
+        <v>24</v>
       </c>
       <c r="L147" s="13"/>
       <c r="M147" s="13"/>
@@ -5120,16 +5141,16 @@
     </row>
     <row r="148" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
       <c r="F148" s="9" t="n">
-        <v>273104907</v>
+        <v>485637054</v>
       </c>
       <c r="G148" s="9" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H148" s="10" t="s">
         <v>14</v>
@@ -5141,7 +5162,7 @@
         <v>16</v>
       </c>
       <c r="K148" s="10" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="L148" s="10"/>
       <c r="M148" s="10"/>
@@ -5149,16 +5170,16 @@
     </row>
     <row r="149" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="11" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C149" s="11"/>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
       <c r="F149" s="12" t="n">
-        <v>485444948</v>
+        <v>291464876</v>
       </c>
       <c r="G149" s="12" t="s">
-        <v>235</v>
+        <v>130</v>
       </c>
       <c r="H149" s="13" t="s">
         <v>14</v>
@@ -5170,7 +5191,7 @@
         <v>16</v>
       </c>
       <c r="K149" s="13" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="L149" s="13"/>
       <c r="M149" s="13"/>
@@ -5180,16 +5201,16 @@
     </row>
     <row r="150" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
       <c r="E150" s="8"/>
       <c r="F150" s="9" t="n">
-        <v>485637054</v>
+        <v>469841399</v>
       </c>
       <c r="G150" s="9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H150" s="10" t="s">
         <v>14</v>
@@ -5201,7 +5222,7 @@
         <v>16</v>
       </c>
       <c r="K150" s="10" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="L150" s="10"/>
       <c r="M150" s="10"/>
@@ -5209,13 +5230,13 @@
     </row>
     <row r="151" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="11" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C151" s="11"/>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
       <c r="F151" s="12" t="n">
-        <v>291464876</v>
+        <v>44229952</v>
       </c>
       <c r="G151" s="12" t="s">
         <v>130</v>
@@ -5230,7 +5251,7 @@
         <v>16</v>
       </c>
       <c r="K151" s="13" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="L151" s="13"/>
       <c r="M151" s="13"/>
@@ -5240,16 +5261,16 @@
     </row>
     <row r="152" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
       <c r="E152" s="8"/>
       <c r="F152" s="9" t="n">
-        <v>469841399</v>
+        <v>393439422</v>
       </c>
       <c r="G152" s="9" t="s">
-        <v>240</v>
+        <v>130</v>
       </c>
       <c r="H152" s="10" t="s">
         <v>14</v>
@@ -5261,7 +5282,7 @@
         <v>16</v>
       </c>
       <c r="K152" s="10" t="s">
-        <v>24</v>
+        <v>242</v>
       </c>
       <c r="L152" s="10"/>
       <c r="M152" s="10"/>
@@ -5269,16 +5290,16 @@
     </row>
     <row r="153" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
       <c r="F153" s="12" t="n">
-        <v>44229952</v>
+        <v>305463917</v>
       </c>
       <c r="G153" s="12" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
       <c r="H153" s="13" t="s">
         <v>14</v>
@@ -5290,7 +5311,7 @@
         <v>16</v>
       </c>
       <c r="K153" s="13" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="L153" s="13"/>
       <c r="M153" s="13"/>
@@ -5300,16 +5321,16 @@
     </row>
     <row r="154" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="8" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
       <c r="E154" s="8"/>
       <c r="F154" s="9" t="n">
-        <v>393439422</v>
+        <v>457968501</v>
       </c>
       <c r="G154" s="9" t="s">
-        <v>130</v>
+        <v>246</v>
       </c>
       <c r="H154" s="10" t="s">
         <v>14</v>
@@ -5321,7 +5342,7 @@
         <v>16</v>
       </c>
       <c r="K154" s="10" t="s">
-        <v>243</v>
+        <v>24</v>
       </c>
       <c r="L154" s="10"/>
       <c r="M154" s="10"/>
@@ -5329,16 +5350,16 @@
     </row>
     <row r="155" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="11" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
       <c r="F155" s="12" t="n">
-        <v>305463917</v>
+        <v>496060553</v>
       </c>
       <c r="G155" s="12" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H155" s="13" t="s">
         <v>14</v>
@@ -5350,7 +5371,7 @@
         <v>16</v>
       </c>
       <c r="K155" s="13" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="L155" s="13"/>
       <c r="M155" s="13"/>
@@ -5360,16 +5381,16 @@
     </row>
     <row r="156" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="8" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
       <c r="E156" s="8"/>
       <c r="F156" s="9" t="n">
-        <v>457968501</v>
+        <v>446001425</v>
       </c>
       <c r="G156" s="9" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H156" s="10" t="s">
         <v>14</v>
@@ -5389,16 +5410,16 @@
     </row>
     <row r="157" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="11" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
       <c r="F157" s="12" t="n">
-        <v>496060553</v>
+        <v>296553831</v>
       </c>
       <c r="G157" s="12" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H157" s="13" t="s">
         <v>14</v>
@@ -5410,7 +5431,7 @@
         <v>16</v>
       </c>
       <c r="K157" s="13" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="L157" s="13"/>
       <c r="M157" s="13"/>
@@ -5420,16 +5441,16 @@
     </row>
     <row r="158" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="8" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
       <c r="F158" s="9" t="n">
-        <v>446001425</v>
+        <v>38598435</v>
       </c>
       <c r="G158" s="9" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="H158" s="10" t="s">
         <v>14</v>
@@ -5441,7 +5462,7 @@
         <v>16</v>
       </c>
       <c r="K158" s="10" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="L158" s="10"/>
       <c r="M158" s="10"/>
@@ -5449,16 +5470,16 @@
     </row>
     <row r="159" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="11" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C159" s="11"/>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
       <c r="F159" s="12" t="n">
-        <v>296553831</v>
+        <v>421311023</v>
       </c>
       <c r="G159" s="12" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H159" s="13" t="s">
         <v>14</v>
@@ -5470,7 +5491,7 @@
         <v>16</v>
       </c>
       <c r="K159" s="13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L159" s="13"/>
       <c r="M159" s="13"/>
@@ -5480,16 +5501,16 @@
     </row>
     <row r="160" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="8" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="8"/>
       <c r="E160" s="8"/>
       <c r="F160" s="9" t="n">
-        <v>38598435</v>
+        <v>447142599</v>
       </c>
       <c r="G160" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H160" s="10" t="s">
         <v>14</v>
@@ -5501,7 +5522,7 @@
         <v>16</v>
       </c>
       <c r="K160" s="10" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="L160" s="10"/>
       <c r="M160" s="10"/>
@@ -5509,16 +5530,16 @@
     </row>
     <row r="161" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="11" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
       <c r="F161" s="12" t="n">
-        <v>421311023</v>
+        <v>427359750</v>
       </c>
       <c r="G161" s="12" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H161" s="13" t="s">
         <v>14</v>
@@ -5530,7 +5551,7 @@
         <v>16</v>
       </c>
       <c r="K161" s="13" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L161" s="13"/>
       <c r="M161" s="13"/>
@@ -5540,16 +5561,16 @@
     </row>
     <row r="162" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="8"/>
       <c r="E162" s="8"/>
       <c r="F162" s="9" t="n">
-        <v>447142599</v>
+        <v>25633126</v>
       </c>
       <c r="G162" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H162" s="10" t="s">
         <v>14</v>
@@ -5561,123 +5582,49 @@
         <v>16</v>
       </c>
       <c r="K162" s="10" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="L162" s="10"/>
       <c r="M162" s="10"/>
       <c r="N162" s="10"/>
     </row>
-    <row r="163" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C163" s="11"/>
-      <c r="D163" s="11"/>
-      <c r="E163" s="11"/>
-      <c r="F163" s="12" t="n">
-        <v>427359750</v>
-      </c>
-      <c r="G163" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="H163" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I163" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J163" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K163" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L163" s="13"/>
-      <c r="M163" s="13"/>
-      <c r="N163" s="13"/>
-      <c r="O163" s="14"/>
-      <c r="P163" s="14"/>
-    </row>
-    <row r="164" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="8" t="s">
+    <row r="163" customFormat="false" ht="27.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B163" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="C164" s="8"/>
-      <c r="D164" s="8"/>
-      <c r="E164" s="8"/>
-      <c r="F164" s="9" t="n">
-        <v>25633126</v>
-      </c>
-      <c r="G164" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="H164" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I164" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J164" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K164" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="L164" s="10"/>
-      <c r="M164" s="10"/>
-      <c r="N164" s="10"/>
-    </row>
-    <row r="165" customFormat="false" ht="1.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="7"/>
-      <c r="C165" s="7"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
-      <c r="G165" s="7"/>
-      <c r="H165" s="7"/>
-      <c r="I165" s="7"/>
-      <c r="J165" s="7"/>
-      <c r="K165" s="7"/>
-      <c r="L165" s="7"/>
-      <c r="M165" s="7"/>
-      <c r="N165" s="7"/>
-      <c r="O165" s="7"/>
-      <c r="P165" s="7"/>
-    </row>
-    <row r="166" customFormat="false" ht="27.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="18" t="s">
+      <c r="C163" s="18"/>
+      <c r="D163" s="18"/>
+      <c r="E163" s="18"/>
+      <c r="F163" s="18"/>
+      <c r="G163" s="18"/>
+      <c r="H163" s="18"/>
+      <c r="I163" s="18"/>
+      <c r="J163" s="18"/>
+      <c r="K163" s="18"/>
+      <c r="L163" s="18"/>
+      <c r="M163" s="18"/>
+      <c r="N163" s="18"/>
+      <c r="O163" s="18"/>
+      <c r="P163" s="18"/>
+    </row>
+    <row r="164" customFormat="false" ht="165.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="10.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B165" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="C166" s="18"/>
-      <c r="D166" s="18"/>
-      <c r="E166" s="18"/>
-      <c r="F166" s="18"/>
-      <c r="G166" s="18"/>
-      <c r="H166" s="18"/>
-      <c r="I166" s="18"/>
-      <c r="J166" s="18"/>
-      <c r="K166" s="18"/>
-      <c r="L166" s="18"/>
-      <c r="M166" s="18"/>
-      <c r="N166" s="18"/>
-      <c r="O166" s="18"/>
-      <c r="P166" s="18"/>
-    </row>
-    <row r="167" customFormat="false" ht="165.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="10.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="C168" s="15"/>
-      <c r="L168" s="16" t="s">
+      <c r="C165" s="15"/>
+      <c r="L165" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M168" s="16"/>
-      <c r="N168" s="16"/>
-      <c r="O168" s="16"/>
-      <c r="P168" s="16"/>
-    </row>
-    <row r="169" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="M165" s="16"/>
+      <c r="N165" s="16"/>
+      <c r="O165" s="16"/>
+      <c r="P165" s="16"/>
+    </row>
+    <row r="166" customFormat="false" ht="0.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="262">
     <mergeCell ref="E4:L4"/>
@@ -5771,15 +5718,17 @@
     <mergeCell ref="K54:N54"/>
     <mergeCell ref="B55:E55"/>
     <mergeCell ref="K55:N55"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="L58:P59"/>
-    <mergeCell ref="E63:L63"/>
-    <mergeCell ref="E65:L66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="L57:P58"/>
+    <mergeCell ref="E62:L62"/>
+    <mergeCell ref="E64:L65"/>
+    <mergeCell ref="B68:P68"/>
     <mergeCell ref="B69:P69"/>
-    <mergeCell ref="B70:P70"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="K72:N72"/>
     <mergeCell ref="B73:E73"/>
     <mergeCell ref="K73:N73"/>
     <mergeCell ref="B74:E74"/>
@@ -5862,17 +5811,19 @@
     <mergeCell ref="K112:N112"/>
     <mergeCell ref="B113:E113"/>
     <mergeCell ref="K113:N113"/>
-    <mergeCell ref="B114:E114"/>
-    <mergeCell ref="K114:N114"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="L117:P118"/>
-    <mergeCell ref="E122:L122"/>
-    <mergeCell ref="E124:L125"/>
-    <mergeCell ref="B128:P128"/>
-    <mergeCell ref="B129:P129"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="L115:P116"/>
+    <mergeCell ref="E120:L120"/>
+    <mergeCell ref="E122:L123"/>
+    <mergeCell ref="B126:P126"/>
+    <mergeCell ref="B127:P127"/>
+    <mergeCell ref="B128:E128"/>
+    <mergeCell ref="K128:N128"/>
+    <mergeCell ref="O128:P128"/>
     <mergeCell ref="B130:E130"/>
     <mergeCell ref="K130:N130"/>
-    <mergeCell ref="O130:P130"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="K131:N131"/>
     <mergeCell ref="B132:E132"/>
     <mergeCell ref="K132:N132"/>
     <mergeCell ref="B133:E133"/>
@@ -5935,13 +5886,9 @@
     <mergeCell ref="K161:N161"/>
     <mergeCell ref="B162:E162"/>
     <mergeCell ref="K162:N162"/>
-    <mergeCell ref="B163:E163"/>
-    <mergeCell ref="K163:N163"/>
-    <mergeCell ref="B164:E164"/>
-    <mergeCell ref="K164:N164"/>
-    <mergeCell ref="B166:P166"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="L168:P169"/>
+    <mergeCell ref="B163:P163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="L165:P166"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5951,9 +5898,9 @@
     <oddFooter/>
   </headerFooter>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="59" man="true" max="16383" min="0"/>
-    <brk id="118" man="true" max="16383" min="0"/>
-    <brk id="169" man="true" max="16383" min="0"/>
+    <brk id="58" man="true" max="16383" min="0"/>
+    <brk id="116" man="true" max="16383" min="0"/>
+    <brk id="166" man="true" max="16383" min="0"/>
   </rowBreaks>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>